<commit_message>
outputting audio features into excel
</commit_message>
<xml_diff>
--- a/spotipy/output.xlsx
+++ b/spotipy/output.xlsx
@@ -13,10 +13,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+  <si>
+    <t>Starboy</t>
+  </si>
+  <si>
+    <t>One Dance</t>
+  </si>
+  <si>
+    <t>Too Good</t>
+  </si>
+  <si>
+    <t>Fix You</t>
+  </si>
+  <si>
+    <t>[{'acousticness': 0.169, 'instrumentalness': 5.49e-06, 'speechiness': 0.281, 'tempo': 186.041, 'id': '2IY7eOUDjw2ArKYxKa2jXc', 'track_href': 'https://api.spotify.com/v1/tracks/2IY7eOUDjw2ArKYxKa2jXc', 'time_signature': 4, 'duration_ms': 230467, 'key': 7, 'valence': 0.477, 'danceability': 0.682, 'uri': 'spotify:track:2IY7eOUDjw2ArKYxKa2jXc', 'mode': 1, 'energy': 0.592, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/2IY7eOUDjw2ArKYxKa2jXc', 'loudness': -7.033, 'type': 'audio_features', 'liveness': 0.136}]</t>
+  </si>
+  <si>
+    <t>[{'acousticness': 0.00902, 'instrumentalness': 0.00246, 'speechiness': 0.0522, 'tempo': 103.981, 'id': '12VWzyPDBCc8fqeWCAfNwR', 'track_href': 'https://api.spotify.com/v1/tracks/12VWzyPDBCc8fqeWCAfNwR', 'time_signature': 4, 'duration_ms': 173987, 'key': 1, 'valence': 0.378, 'danceability': 0.785, 'uri': 'spotify:track:12VWzyPDBCc8fqeWCAfNwR', 'mode': 1, 'energy': 0.617, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/12VWzyPDBCc8fqeWCAfNwR', 'loudness': -5.871, 'type': 'audio_features', 'liveness': 0.351}]</t>
+  </si>
+  <si>
+    <t>[{'acousticness': 0.0606, 'instrumentalness': 7.05e-05, 'speechiness': 0.118, 'tempo': 117.984, 'id': '7fJtPlEZKxu6gvkfBFc5tW', 'track_href': 'https://api.spotify.com/v1/tracks/7fJtPlEZKxu6gvkfBFc5tW', 'time_signature': 4, 'duration_ms': 263373, 'key': 7, 'valence': 0.391, 'danceability': 0.804, 'uri': 'spotify:track:7fJtPlEZKxu6gvkfBFc5tW', 'mode': 1, 'energy': 0.65, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7fJtPlEZKxu6gvkfBFc5tW', 'loudness': -7.79, 'type': 'audio_features', 'liveness': 0.102}]</t>
+  </si>
+  <si>
+    <t>[{'acousticness': 0.163, 'instrumentalness': 0.00195, 'speechiness': 0.0338, 'tempo': 138.265, 'id': '7LVHVU3tWfcxj5aiPFEW4Q', 'track_href': 'https://api.spotify.com/v1/tracks/7LVHVU3tWfcxj5aiPFEW4Q', 'time_signature': 4, 'duration_ms': 295533, 'key': 3, 'valence': 0.122, 'danceability': 0.209, 'uri': 'spotify:track:7LVHVU3tWfcxj5aiPFEW4Q', 'mode': 1, 'energy': 0.418, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7LVHVU3tWfcxj5aiPFEW4Q', 'loudness': -8.74, 'type': 'audio_features', 'liveness': 0.113}]</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +77,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +395,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified input file and outupt to excel
</commit_message>
<xml_diff>
--- a/spotipy/output.xlsx
+++ b/spotipy/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Starboy</t>
   </si>
@@ -28,16 +28,46 @@
     <t>Fix You</t>
   </si>
   <si>
-    <t>[{'acousticness': 0.169, 'instrumentalness': 5.49e-06, 'speechiness': 0.281, 'tempo': 186.041, 'id': '2IY7eOUDjw2ArKYxKa2jXc', 'track_href': 'https://api.spotify.com/v1/tracks/2IY7eOUDjw2ArKYxKa2jXc', 'time_signature': 4, 'duration_ms': 230467, 'key': 7, 'valence': 0.477, 'danceability': 0.682, 'uri': 'spotify:track:2IY7eOUDjw2ArKYxKa2jXc', 'mode': 1, 'energy': 0.592, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/2IY7eOUDjw2ArKYxKa2jXc', 'loudness': -7.033, 'type': 'audio_features', 'liveness': 0.136}]</t>
-  </si>
-  <si>
-    <t>[{'acousticness': 0.00902, 'instrumentalness': 0.00246, 'speechiness': 0.0522, 'tempo': 103.981, 'id': '12VWzyPDBCc8fqeWCAfNwR', 'track_href': 'https://api.spotify.com/v1/tracks/12VWzyPDBCc8fqeWCAfNwR', 'time_signature': 4, 'duration_ms': 173987, 'key': 1, 'valence': 0.378, 'danceability': 0.785, 'uri': 'spotify:track:12VWzyPDBCc8fqeWCAfNwR', 'mode': 1, 'energy': 0.617, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/12VWzyPDBCc8fqeWCAfNwR', 'loudness': -5.871, 'type': 'audio_features', 'liveness': 0.351}]</t>
-  </si>
-  <si>
-    <t>[{'acousticness': 0.0606, 'instrumentalness': 7.05e-05, 'speechiness': 0.118, 'tempo': 117.984, 'id': '7fJtPlEZKxu6gvkfBFc5tW', 'track_href': 'https://api.spotify.com/v1/tracks/7fJtPlEZKxu6gvkfBFc5tW', 'time_signature': 4, 'duration_ms': 263373, 'key': 7, 'valence': 0.391, 'danceability': 0.804, 'uri': 'spotify:track:7fJtPlEZKxu6gvkfBFc5tW', 'mode': 1, 'energy': 0.65, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7fJtPlEZKxu6gvkfBFc5tW', 'loudness': -7.79, 'type': 'audio_features', 'liveness': 0.102}]</t>
-  </si>
-  <si>
-    <t>[{'acousticness': 0.163, 'instrumentalness': 0.00195, 'speechiness': 0.0338, 'tempo': 138.265, 'id': '7LVHVU3tWfcxj5aiPFEW4Q', 'track_href': 'https://api.spotify.com/v1/tracks/7LVHVU3tWfcxj5aiPFEW4Q', 'time_signature': 4, 'duration_ms': 295533, 'key': 3, 'valence': 0.122, 'danceability': 0.209, 'uri': 'spotify:track:7LVHVU3tWfcxj5aiPFEW4Q', 'mode': 1, 'energy': 0.418, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7LVHVU3tWfcxj5aiPFEW4Q', 'loudness': -8.74, 'type': 'audio_features', 'liveness': 0.113}]</t>
+    <t>Hold On, We're Going Home</t>
+  </si>
+  <si>
+    <t>I Took A Pill In Ibiza - Seeb Remix</t>
+  </si>
+  <si>
+    <t>Love Yourself</t>
+  </si>
+  <si>
+    <t>Side To Side</t>
+  </si>
+  <si>
+    <t>Truffle Butter</t>
+  </si>
+  <si>
+    <t>[{'key': 7, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/2IY7eOUDjw2ArKYxKa2jXc', 'valence': 0.477, 'energy': 0.592, 'liveness': 0.136, 'speechiness': 0.281, 'loudness': -7.033, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/2IY7eOUDjw2ArKYxKa2jXc', 'danceability': 0.682, 'acousticness': 0.169, 'tempo': 186.041, 'duration_ms': 230467, 'id': '2IY7eOUDjw2ArKYxKa2jXc', 'instrumentalness': 5.49e-06, 'time_signature': 4, 'uri': 'spotify:track:2IY7eOUDjw2ArKYxKa2jXc'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 1, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/12VWzyPDBCc8fqeWCAfNwR', 'valence': 0.378, 'energy': 0.617, 'liveness': 0.351, 'speechiness': 0.0522, 'loudness': -5.871, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/12VWzyPDBCc8fqeWCAfNwR', 'danceability': 0.785, 'acousticness': 0.00902, 'tempo': 103.981, 'duration_ms': 173987, 'id': '12VWzyPDBCc8fqeWCAfNwR', 'instrumentalness': 0.00246, 'time_signature': 4, 'uri': 'spotify:track:12VWzyPDBCc8fqeWCAfNwR'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 7, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/7fJtPlEZKxu6gvkfBFc5tW', 'valence': 0.391, 'energy': 0.65, 'liveness': 0.102, 'speechiness': 0.118, 'loudness': -7.79, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7fJtPlEZKxu6gvkfBFc5tW', 'danceability': 0.804, 'acousticness': 0.0606, 'tempo': 117.984, 'duration_ms': 263373, 'id': '7fJtPlEZKxu6gvkfBFc5tW', 'instrumentalness': 7.05e-05, 'time_signature': 4, 'uri': 'spotify:track:7fJtPlEZKxu6gvkfBFc5tW'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 3, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/7LVHVU3tWfcxj5aiPFEW4Q', 'valence': 0.122, 'energy': 0.418, 'liveness': 0.113, 'speechiness': 0.0338, 'loudness': -8.74, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7LVHVU3tWfcxj5aiPFEW4Q', 'danceability': 0.209, 'acousticness': 0.163, 'tempo': 138.265, 'duration_ms': 295533, 'id': '7LVHVU3tWfcxj5aiPFEW4Q', 'instrumentalness': 0.00195, 'time_signature': 4, 'uri': 'spotify:track:7LVHVU3tWfcxj5aiPFEW4Q'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 6, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/14Rcq31SafFBHNEwXrtR2B', 'valence': 0.287, 'energy': 0.407, 'liveness': 0.0705, 'speechiness': 0.0907, 'loudness': -7.442, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/14Rcq31SafFBHNEwXrtR2B', 'danceability': 0.772, 'acousticness': 0.00349, 'tempo': 100.006, 'duration_ms': 227880, 'id': '14Rcq31SafFBHNEwXrtR2B', 'instrumentalness': 2.4e-05, 'time_signature': 4, 'uri': 'spotify:track:14Rcq31SafFBHNEwXrtR2B'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 7, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/1MtUq6Wp1eQ8PC6BbPCj8P', 'valence': 0.697, 'energy': 0.725, 'liveness': 0.0864, 'speechiness': 0.12, 'loudness': -6.588, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/1MtUq6Wp1eQ8PC6BbPCj8P', 'danceability': 0.665, 'acousticness': 0.034, 'tempo': 101.96, 'duration_ms': 197933, 'id': '1MtUq6Wp1eQ8PC6BbPCj8P', 'instrumentalness': 9.17e-06, 'time_signature': 4, 'uri': 'spotify:track:1MtUq6Wp1eQ8PC6BbPCj8P'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 4, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/50kpGaPAhYJ3sGmk6vplg0', 'valence': 0.559, 'energy': 0.376, 'liveness': 0.285, 'speechiness': 0.453, 'loudness': -9.954, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/50kpGaPAhYJ3sGmk6vplg0', 'danceability': 0.607, 'acousticness': 0.856, 'tempo': 102.541, 'duration_ms': 233720, 'id': '50kpGaPAhYJ3sGmk6vplg0', 'instrumentalness': 0, 'time_signature': 4, 'uri': 'spotify:track:50kpGaPAhYJ3sGmk6vplg0'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 6, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/1pKeFVVUOPjFsOABub0OaV', 'valence': 0.624, 'energy': 0.728, 'liveness': 0.328, 'speechiness': 0.232, 'loudness': -5.914, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/1pKeFVVUOPjFsOABub0OaV', 'danceability': 0.65, 'acousticness': 0.0373, 'tempo': 159.167, 'duration_ms': 226160, 'id': '1pKeFVVUOPjFsOABub0OaV', 'instrumentalness': 0, 'time_signature': 4, 'uri': 'spotify:track:1pKeFVVUOPjFsOABub0OaV'}]</t>
+  </si>
+  <si>
+    <t>[{'key': 10, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/3keUgTGEoZJt0QkzTB6kHg', 'valence': 0.511, 'energy': 0.672, 'liveness': 0.12, 'speechiness': 0.0479, 'loudness': -6.875, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/3keUgTGEoZJt0QkzTB6kHg', 'danceability': 0.896, 'acousticness': 0.0525, 'tempo': 105.098, 'duration_ms': 219227, 'id': '3keUgTGEoZJt0QkzTB6kHg', 'instrumentalness': 3.14e-05, 'time_signature': 4, 'uri': 'spotify:track:3keUgTGEoZJt0QkzTB6kHg'}]</t>
   </si>
 </sst>
 </file>
@@ -395,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,7 +447,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -428,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -439,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -450,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -461,7 +491,62 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
         <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added popularity of track. Added functionality to split attributes into excel columns
</commit_message>
<xml_diff>
--- a/spotipy/output.xlsx
+++ b/spotipy/output.xlsx
@@ -14,7 +14,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>song</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>dance</t>
+  </si>
+  <si>
+    <t>liveness</t>
+  </si>
+  <si>
+    <t>valence</t>
+  </si>
+  <si>
+    <t>tempo</t>
+  </si>
+  <si>
+    <t>instrumental</t>
+  </si>
+  <si>
+    <t>acoustic</t>
+  </si>
+  <si>
+    <t>popularity</t>
+  </si>
   <si>
     <t>Starboy</t>
   </si>
@@ -28,6 +55,9 @@
     <t>Fix You</t>
   </si>
   <si>
+    <t>Trust Issues Drake</t>
+  </si>
+  <si>
     <t>Hold On, We're Going Home</t>
   </si>
   <si>
@@ -41,33 +71,6 @@
   </si>
   <si>
     <t>Truffle Butter</t>
-  </si>
-  <si>
-    <t>[{'key': 7, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/2IY7eOUDjw2ArKYxKa2jXc', 'valence': 0.477, 'energy': 0.592, 'liveness': 0.136, 'speechiness': 0.281, 'loudness': -7.033, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/2IY7eOUDjw2ArKYxKa2jXc', 'danceability': 0.682, 'acousticness': 0.169, 'tempo': 186.041, 'duration_ms': 230467, 'id': '2IY7eOUDjw2ArKYxKa2jXc', 'instrumentalness': 5.49e-06, 'time_signature': 4, 'uri': 'spotify:track:2IY7eOUDjw2ArKYxKa2jXc'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 1, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/12VWzyPDBCc8fqeWCAfNwR', 'valence': 0.378, 'energy': 0.617, 'liveness': 0.351, 'speechiness': 0.0522, 'loudness': -5.871, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/12VWzyPDBCc8fqeWCAfNwR', 'danceability': 0.785, 'acousticness': 0.00902, 'tempo': 103.981, 'duration_ms': 173987, 'id': '12VWzyPDBCc8fqeWCAfNwR', 'instrumentalness': 0.00246, 'time_signature': 4, 'uri': 'spotify:track:12VWzyPDBCc8fqeWCAfNwR'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 7, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/7fJtPlEZKxu6gvkfBFc5tW', 'valence': 0.391, 'energy': 0.65, 'liveness': 0.102, 'speechiness': 0.118, 'loudness': -7.79, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7fJtPlEZKxu6gvkfBFc5tW', 'danceability': 0.804, 'acousticness': 0.0606, 'tempo': 117.984, 'duration_ms': 263373, 'id': '7fJtPlEZKxu6gvkfBFc5tW', 'instrumentalness': 7.05e-05, 'time_signature': 4, 'uri': 'spotify:track:7fJtPlEZKxu6gvkfBFc5tW'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 3, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/7LVHVU3tWfcxj5aiPFEW4Q', 'valence': 0.122, 'energy': 0.418, 'liveness': 0.113, 'speechiness': 0.0338, 'loudness': -8.74, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/7LVHVU3tWfcxj5aiPFEW4Q', 'danceability': 0.209, 'acousticness': 0.163, 'tempo': 138.265, 'duration_ms': 295533, 'id': '7LVHVU3tWfcxj5aiPFEW4Q', 'instrumentalness': 0.00195, 'time_signature': 4, 'uri': 'spotify:track:7LVHVU3tWfcxj5aiPFEW4Q'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 6, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/14Rcq31SafFBHNEwXrtR2B', 'valence': 0.287, 'energy': 0.407, 'liveness': 0.0705, 'speechiness': 0.0907, 'loudness': -7.442, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/14Rcq31SafFBHNEwXrtR2B', 'danceability': 0.772, 'acousticness': 0.00349, 'tempo': 100.006, 'duration_ms': 227880, 'id': '14Rcq31SafFBHNEwXrtR2B', 'instrumentalness': 2.4e-05, 'time_signature': 4, 'uri': 'spotify:track:14Rcq31SafFBHNEwXrtR2B'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 7, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/1MtUq6Wp1eQ8PC6BbPCj8P', 'valence': 0.697, 'energy': 0.725, 'liveness': 0.0864, 'speechiness': 0.12, 'loudness': -6.588, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/1MtUq6Wp1eQ8PC6BbPCj8P', 'danceability': 0.665, 'acousticness': 0.034, 'tempo': 101.96, 'duration_ms': 197933, 'id': '1MtUq6Wp1eQ8PC6BbPCj8P', 'instrumentalness': 9.17e-06, 'time_signature': 4, 'uri': 'spotify:track:1MtUq6Wp1eQ8PC6BbPCj8P'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 4, 'mode': 1, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/50kpGaPAhYJ3sGmk6vplg0', 'valence': 0.559, 'energy': 0.376, 'liveness': 0.285, 'speechiness': 0.453, 'loudness': -9.954, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/50kpGaPAhYJ3sGmk6vplg0', 'danceability': 0.607, 'acousticness': 0.856, 'tempo': 102.541, 'duration_ms': 233720, 'id': '50kpGaPAhYJ3sGmk6vplg0', 'instrumentalness': 0, 'time_signature': 4, 'uri': 'spotify:track:50kpGaPAhYJ3sGmk6vplg0'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 6, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/1pKeFVVUOPjFsOABub0OaV', 'valence': 0.624, 'energy': 0.728, 'liveness': 0.328, 'speechiness': 0.232, 'loudness': -5.914, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/1pKeFVVUOPjFsOABub0OaV', 'danceability': 0.65, 'acousticness': 0.0373, 'tempo': 159.167, 'duration_ms': 226160, 'id': '1pKeFVVUOPjFsOABub0OaV', 'instrumentalness': 0, 'time_signature': 4, 'uri': 'spotify:track:1pKeFVVUOPjFsOABub0OaV'}]</t>
-  </si>
-  <si>
-    <t>[{'key': 10, 'mode': 0, 'type': 'audio_features', 'track_href': 'https://api.spotify.com/v1/tracks/3keUgTGEoZJt0QkzTB6kHg', 'valence': 0.511, 'energy': 0.672, 'liveness': 0.12, 'speechiness': 0.0479, 'loudness': -6.875, 'analysis_url': 'https://api.spotify.com/v1/audio-analysis/3keUgTGEoZJt0QkzTB6kHg', 'danceability': 0.896, 'acousticness': 0.0525, 'tempo': 105.098, 'duration_ms': 219227, 'id': '3keUgTGEoZJt0QkzTB6kHg', 'instrumentalness': 3.14e-05, 'time_signature': 4, 'uri': 'spotify:track:3keUgTGEoZJt0QkzTB6kHg'}]</t>
   </si>
 </sst>
 </file>
@@ -425,128 +428,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1">
+    <row r="1" spans="1:10">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2">
+        <v>0.592</v>
+      </c>
+      <c r="D2">
+        <v>0.6820000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.136</v>
+      </c>
+      <c r="F2">
+        <v>0.477</v>
+      </c>
+      <c r="G2">
+        <v>186.041</v>
+      </c>
+      <c r="H2">
+        <v>5.49e-06</v>
+      </c>
+      <c r="I2">
+        <v>0.169</v>
+      </c>
+      <c r="J2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3">
+        <v>0.617</v>
+      </c>
+      <c r="D3">
+        <v>0.785</v>
+      </c>
+      <c r="E3">
+        <v>0.351</v>
+      </c>
+      <c r="F3">
+        <v>0.378</v>
+      </c>
+      <c r="G3">
+        <v>103.981</v>
+      </c>
+      <c r="H3">
+        <v>0.00246</v>
+      </c>
+      <c r="I3">
+        <v>0.00902</v>
+      </c>
+      <c r="J3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4">
+        <v>0.65</v>
+      </c>
+      <c r="D4">
+        <v>0.804</v>
+      </c>
+      <c r="E4">
+        <v>0.102</v>
+      </c>
+      <c r="F4">
+        <v>0.391</v>
+      </c>
+      <c r="G4">
+        <v>117.984</v>
+      </c>
+      <c r="H4">
+        <v>7.050000000000001e-05</v>
+      </c>
+      <c r="I4">
+        <v>0.0606</v>
+      </c>
+      <c r="J4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5">
+        <v>0.418</v>
+      </c>
+      <c r="D5">
+        <v>0.209</v>
+      </c>
+      <c r="E5">
+        <v>0.113</v>
+      </c>
+      <c r="F5">
+        <v>0.122</v>
+      </c>
+      <c r="G5">
+        <v>138.265</v>
+      </c>
+      <c r="H5">
+        <v>0.00195</v>
+      </c>
+      <c r="I5">
+        <v>0.163</v>
+      </c>
+      <c r="J5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0.407</v>
+      </c>
+      <c r="D7">
+        <v>0.772</v>
+      </c>
+      <c r="E7">
+        <v>0.07049999999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.287</v>
+      </c>
+      <c r="G7">
+        <v>100.006</v>
+      </c>
+      <c r="H7">
+        <v>2.4e-05</v>
+      </c>
+      <c r="I7">
+        <v>0.00349</v>
+      </c>
+      <c r="J7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>0.725</v>
+      </c>
+      <c r="D8">
+        <v>0.665</v>
+      </c>
+      <c r="E8">
+        <v>0.0864</v>
+      </c>
+      <c r="F8">
+        <v>0.697</v>
+      </c>
+      <c r="G8">
+        <v>101.96</v>
+      </c>
+      <c r="H8">
+        <v>9.17e-06</v>
+      </c>
+      <c r="I8">
+        <v>0.034</v>
+      </c>
+      <c r="J8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0.376</v>
+      </c>
+      <c r="D9">
+        <v>0.607</v>
+      </c>
+      <c r="E9">
+        <v>0.285</v>
+      </c>
+      <c r="F9">
+        <v>0.5590000000000001</v>
+      </c>
+      <c r="G9">
+        <v>102.541</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.856</v>
+      </c>
+      <c r="J9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0.728</v>
+      </c>
+      <c r="D10">
+        <v>0.65</v>
+      </c>
+      <c r="E10">
+        <v>0.328</v>
+      </c>
+      <c r="F10">
+        <v>0.624</v>
+      </c>
+      <c r="G10">
+        <v>159.167</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.0373</v>
+      </c>
+      <c r="J10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>0.672</v>
+      </c>
+      <c r="D11">
+        <v>0.896</v>
+      </c>
+      <c r="E11">
+        <v>0.12</v>
+      </c>
+      <c r="F11">
+        <v>0.511</v>
+      </c>
+      <c r="G11">
+        <v>105.098</v>
+      </c>
+      <c r="H11">
+        <v>3.14e-05</v>
+      </c>
+      <c r="I11">
+        <v>0.0525</v>
+      </c>
+      <c r="J11">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added genres. added artists. Both are now outputted. Removed nested for loop
</commit_message>
<xml_diff>
--- a/spotipy/output.xlsx
+++ b/spotipy/output.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>song</t>
   </si>
   <si>
+    <t>artist</t>
+  </si>
+  <si>
     <t>energy</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t>popularity</t>
   </si>
   <si>
+    <t>genres</t>
+  </si>
+  <si>
     <t>Starboy</t>
   </si>
   <si>
@@ -71,6 +77,48 @@
   </si>
   <si>
     <t>Truffle Butter</t>
+  </si>
+  <si>
+    <t>The Weeknd</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>Coldplay</t>
+  </si>
+  <si>
+    <t>Mike Posner</t>
+  </si>
+  <si>
+    <t>Justin Bieber</t>
+  </si>
+  <si>
+    <t>Ariana Grande</t>
+  </si>
+  <si>
+    <t>Nicki Minaj</t>
+  </si>
+  <si>
+    <t>['canadian pop', 'pop']</t>
+  </si>
+  <si>
+    <t>['canadian pop', 'hip hop', 'pop rap', 'rap']</t>
+  </si>
+  <si>
+    <t>['permanent wave', 'pop', 'pop christmas', 'rock']</t>
+  </si>
+  <si>
+    <t>['dance pop', 'pop', 'pop rap', 'post-teen pop', 'tropical house']</t>
+  </si>
+  <si>
+    <t>['canadian pop', 'dance pop', 'pop', 'pop christmas', 'post-teen pop']</t>
+  </si>
+  <si>
+    <t>['dance pop', 'pop', 'pop christmas', 'post-teen pop']</t>
+  </si>
+  <si>
+    <t>['dance pop', 'dwn trap', 'hip pop', 'pop', 'pop rap']</t>
   </si>
 </sst>
 </file>
@@ -428,13 +476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,301 +510,361 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
         <v>0.592</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.6820000000000001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.136</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.477</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>186.041</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>5.49e-06</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.169</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
         <v>0.617</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.785</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.351</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.378</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>103.981</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.00246</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.00902</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
         <v>0.65</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.804</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.102</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.391</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>117.984</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>7.050000000000001e-05</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.0606</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
         <v>0.418</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.209</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.113</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.122</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>138.265</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.00195</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.163</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
         <v>0.407</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.772</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.07049999999999999</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.287</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>100.006</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>2.4e-05</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.00349</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
         <v>0.725</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.665</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.0864</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.697</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>101.96</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>9.17e-06</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.034</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
         <v>0.376</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.607</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.285</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.5590000000000001</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>102.541</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.856</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
         <v>0.728</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.65</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.328</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.624</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>159.167</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.0373</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
         <v>0.672</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.896</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.12</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.511</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>105.098</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>3.14e-05</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.0525</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>70</v>
+      </c>
+      <c r="L11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>